<commit_message>
Download mp4 and convert to mp3 successful.
</commit_message>
<xml_diff>
--- a/download.xlsx
+++ b/download.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\download-from-youtube\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\download-from-youtube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584B9678-9957-4F51-A559-FA254E0CAE42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5906AB31-10DA-4D03-8B2F-F14BE6863673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10560" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7365" yWindow="5910" windowWidth="21600" windowHeight="12735" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="112">
   <si>
     <t>Youtube link to download</t>
   </si>
@@ -40,14 +50,329 @@
     <t>https://www.youtube.com/watch?v=PP7WOMnT288</t>
   </si>
   <si>
-    <t>video</t>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>kabira</t>
+  </si>
+  <si>
+    <t>Yeh Jawaani Hai Deewani</t>
+  </si>
+  <si>
+    <t>afreen afreen</t>
+  </si>
+  <si>
+    <t>Coke Studio</t>
+  </si>
+  <si>
+    <t>bakhuda tumhi ho</t>
+  </si>
+  <si>
+    <t>Kismat Konnection</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>Pritam</t>
+  </si>
+  <si>
+    <t>Atif Aslam</t>
+  </si>
+  <si>
+    <t>Rahat Fateh Ali Khan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=60ItHLz5WEA</t>
+  </si>
+  <si>
+    <t>faded</t>
+  </si>
+  <si>
+    <t>Alan Walker</t>
+  </si>
+  <si>
+    <t>Faded</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nYh-n7EOtMA</t>
+  </si>
+  <si>
+    <t>cheap thrills</t>
+  </si>
+  <si>
+    <t>Sia</t>
+  </si>
+  <si>
+    <t>This Is Acting</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1tVL11ULjYY</t>
+  </si>
+  <si>
+    <t>the humma song</t>
+  </si>
+  <si>
+    <t>OK Jaanu</t>
+  </si>
+  <si>
+    <t>A.R. Rahman</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yDv0WSgXJVg</t>
+  </si>
+  <si>
+    <t>senorita</t>
+  </si>
+  <si>
+    <t>Shankar Mahadevan</t>
+  </si>
+  <si>
+    <t>Zindagi Na Milegi Dobara</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zdXiSlRrgWQ</t>
+  </si>
+  <si>
+    <t>naina da kya kasoor</t>
+  </si>
+  <si>
+    <t>Amit Trivedi</t>
+  </si>
+  <si>
+    <t>Andhadhun</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1YqmSp22-60</t>
+  </si>
+  <si>
+    <t>who ladki</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=R0XjwtP_iTY</t>
+  </si>
+  <si>
+    <t>khaabon ke parinday</t>
+  </si>
+  <si>
+    <t>Shankar Ehsaan Loy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=euy__oIUJd4</t>
+  </si>
+  <si>
+    <t>shubharambh</t>
+  </si>
+  <si>
+    <t>Kai Po Che</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YKcmMmJlKNk</t>
+  </si>
+  <si>
+    <t>manja</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gkKcddq0J4U</t>
+  </si>
+  <si>
+    <t>duniya</t>
+  </si>
+  <si>
+    <t>Piyush Mishra</t>
+  </si>
+  <si>
+    <t>Gulaal</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dvgZkm1xWPE</t>
+  </si>
+  <si>
+    <t>viva la vida</t>
+  </si>
+  <si>
+    <t>Coldplay</t>
+  </si>
+  <si>
+    <t>Viva La Vida</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KSwd2fYX9vg</t>
+  </si>
+  <si>
+    <t>allah ke bande</t>
+  </si>
+  <si>
+    <t>Kailash Kher</t>
+  </si>
+  <si>
+    <t>Waisa Bhi Hota Hai - II</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kym6NpYgAc8</t>
+  </si>
+  <si>
+    <t>Shibani Kashyap</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=leECCKm31TA</t>
+  </si>
+  <si>
+    <t>naina</t>
+  </si>
+  <si>
+    <t>Vishal Bhardwaj</t>
+  </si>
+  <si>
+    <t>Omkara</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rfLLnhA3Fi0</t>
+  </si>
+  <si>
+    <t>aaj jaane ki zidd na karo</t>
+  </si>
+  <si>
+    <t>Arjit Singh</t>
+  </si>
+  <si>
+    <t>Monsoon Wedding</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=smn3mDBOUy4</t>
+  </si>
+  <si>
+    <t>jiya re</t>
+  </si>
+  <si>
+    <t>Jab Tak Hai Jaan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CNZMIhckaA0</t>
+  </si>
+  <si>
+    <t>aaoge jab tum</t>
+  </si>
+  <si>
+    <t>Rashid Khan</t>
+  </si>
+  <si>
+    <t>Jab We Met</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=v-eUWdjBgJA</t>
+  </si>
+  <si>
+    <t>saawali si raat</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y7TC2Ef__zw</t>
+  </si>
+  <si>
+    <t>phir le aya dil</t>
+  </si>
+  <si>
+    <t>Barfi</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=O-91jWrOxYk</t>
+  </si>
+  <si>
+    <t>itni si hasi</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=02ossVAJM30</t>
+  </si>
+  <si>
+    <t>main kya karoon</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X_q9IXvt3ro</t>
+  </si>
+  <si>
+    <t>kyon</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gQLMM4VcmXA</t>
+  </si>
+  <si>
+    <t>baatein kuch ankahee</t>
+  </si>
+  <si>
+    <t>Life in a Metro</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PUuhmTrmCuk</t>
+  </si>
+  <si>
+    <t>alvida</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fLdCE9beY6g</t>
+  </si>
+  <si>
+    <t>o meri jaan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Fk3HIOJIjz8</t>
+  </si>
+  <si>
+    <t>in dino</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aw0s2KaoA2Q&amp;list=RDgQLMM4VcmXA&amp;index=9</t>
+  </si>
+  <si>
+    <t>tu aashiqui hai</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>Jhankaar Beats</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZAkr0KFFLLs&amp;list=RDgQLMM4VcmXA&amp;index=10</t>
+  </si>
+  <si>
+    <t>piyu bole</t>
+  </si>
+  <si>
+    <t>Sonu Nigam, Shreya Ghosal</t>
+  </si>
+  <si>
+    <t>Parineeta</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ru_5PA8cwkE&amp;list=RDgQLMM4VcmXA&amp;index=11</t>
+  </si>
+  <si>
+    <t>mitwa</t>
+  </si>
+  <si>
+    <t>Kabhi Alvida Na Kehna</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=g0eO74UmRBs</t>
+  </si>
+  <si>
+    <t>kal ho na ho</t>
+  </si>
+  <si>
+    <t>Sonu Nigam</t>
+  </si>
+  <si>
+    <t>Kal Ho Na Ho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,13 +383,19 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,29 +435,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -408,189 +733,615 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="6" customWidth="1"/>
-    <col min="3" max="4" width="15.33203125" style="2" customWidth="1"/>
-    <col min="5" max="16378" width="9" style="3"/>
+    <col min="1" max="1" width="50.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="5" customWidth="1"/>
+    <col min="6" max="16378" width="9" style="3"/>
+    <col min="16379" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="25.5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="25.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="25.5">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="25.5">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="25.5">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="25.5">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="25.5">
+      <c r="A17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="25.5">
+      <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="25.5">
+      <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="25.5">
+      <c r="A27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="25.5">
+      <c r="A31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="25.5">
+      <c r="A32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="25.5">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:5">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:5">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{7D20D0F7-7ABE-4AEC-B907-1CFC86710409}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Default title is taken from yt.title
</commit_message>
<xml_diff>
--- a/download.xlsx
+++ b/download.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\download-from-youtube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74398AB-63F5-493E-9AC7-671C0FE4977C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6A5E18-6469-4727-ADEE-333ABCCBBCE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10560" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="110">
   <si>
     <t>Youtube link to download</t>
   </si>
@@ -56,15 +56,9 @@
     <t>Yeh Jawaani Hai Deewani</t>
   </si>
   <si>
-    <t>afreen afreen</t>
-  </si>
-  <si>
     <t>Coke Studio</t>
   </si>
   <si>
-    <t>bakhuda tumhi ho</t>
-  </si>
-  <si>
     <t>Kismat Konnection</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>https://www.youtube.com/watch?v=nYh-n7EOtMA</t>
   </si>
   <si>
-    <t>cheap thrills</t>
-  </si>
-  <si>
     <t>Sia</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>https://www.youtube.com/watch?v=zdXiSlRrgWQ</t>
   </si>
   <si>
-    <t>naina da kya kasoor</t>
-  </si>
-  <si>
     <t>Amit Trivedi</t>
   </si>
   <si>
@@ -137,33 +125,21 @@
     <t>https://www.youtube.com/watch?v=R0XjwtP_iTY</t>
   </si>
   <si>
-    <t>khaabon ke parinday</t>
-  </si>
-  <si>
     <t>Shankar Ehsaan Loy</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=euy__oIUJd4</t>
   </si>
   <si>
-    <t>shubharambh</t>
-  </si>
-  <si>
     <t>Kai Po Che</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=YKcmMmJlKNk</t>
   </si>
   <si>
-    <t>manja</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=gkKcddq0J4U</t>
   </si>
   <si>
-    <t>duniya</t>
-  </si>
-  <si>
     <t>Piyush Mishra</t>
   </si>
   <si>
@@ -173,9 +149,6 @@
     <t>https://www.youtube.com/watch?v=dvgZkm1xWPE</t>
   </si>
   <si>
-    <t>viva la vida</t>
-  </si>
-  <si>
     <t>Coldplay</t>
   </si>
   <si>
@@ -185,9 +158,6 @@
     <t>https://www.youtube.com/watch?v=KSwd2fYX9vg</t>
   </si>
   <si>
-    <t>allah ke bande</t>
-  </si>
-  <si>
     <t>Kailash Kher</t>
   </si>
   <si>
@@ -203,9 +173,6 @@
     <t>https://www.youtube.com/watch?v=leECCKm31TA</t>
   </si>
   <si>
-    <t>naina</t>
-  </si>
-  <si>
     <t>Vishal Bhardwaj</t>
   </si>
   <si>
@@ -215,9 +182,6 @@
     <t>https://www.youtube.com/watch?v=rfLLnhA3Fi0</t>
   </si>
   <si>
-    <t>aaj jaane ki zidd na karo</t>
-  </si>
-  <si>
     <t>Arjit Singh</t>
   </si>
   <si>
@@ -233,9 +197,6 @@
     <t>https://www.youtube.com/watch?v=CNZMIhckaA0</t>
   </si>
   <si>
-    <t>aaoge jab tum</t>
-  </si>
-  <si>
     <t>Rashid Khan</t>
   </si>
   <si>
@@ -245,69 +206,39 @@
     <t>https://www.youtube.com/watch?v=v-eUWdjBgJA</t>
   </si>
   <si>
-    <t>saawali si raat</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=y7TC2Ef__zw</t>
   </si>
   <si>
-    <t>phir le aya dil</t>
-  </si>
-  <si>
     <t>Barfi</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=O-91jWrOxYk</t>
   </si>
   <si>
-    <t>itni si hasi</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=02ossVAJM30</t>
   </si>
   <si>
-    <t>main kya karoon</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=X_q9IXvt3ro</t>
   </si>
   <si>
-    <t>kyon</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=gQLMM4VcmXA</t>
   </si>
   <si>
-    <t>baatein kuch ankahee</t>
-  </si>
-  <si>
     <t>Life in a Metro</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=PUuhmTrmCuk</t>
   </si>
   <si>
-    <t>alvida</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=fLdCE9beY6g</t>
   </si>
   <si>
-    <t>o meri jaan</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=Fk3HIOJIjz8</t>
   </si>
   <si>
-    <t>in dino</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=aw0s2KaoA2Q&amp;list=RDgQLMM4VcmXA&amp;index=9</t>
   </si>
   <si>
-    <t>tu aashiqui hai</t>
-  </si>
-  <si>
     <t>KK</t>
   </si>
   <si>
@@ -317,9 +248,6 @@
     <t>https://www.youtube.com/watch?v=ZAkr0KFFLLs&amp;list=RDgQLMM4VcmXA&amp;index=10</t>
   </si>
   <si>
-    <t>piyu bole</t>
-  </si>
-  <si>
     <t>Sonu Nigam, Shreya Ghosal</t>
   </si>
   <si>
@@ -329,27 +257,18 @@
     <t>https://www.youtube.com/watch?v=ru_5PA8cwkE&amp;list=RDgQLMM4VcmXA&amp;index=11</t>
   </si>
   <si>
-    <t>mitwa</t>
-  </si>
-  <si>
     <t>Kabhi Alvida Na Kehna</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=g0eO74UmRBs</t>
   </si>
   <si>
-    <t>kal ho na ho</t>
-  </si>
-  <si>
     <t>Sonu Nigam</t>
   </si>
   <si>
     <t>Kal Ho Na Ho</t>
   </si>
   <si>
-    <t>sajna aa bhi ja</t>
-  </si>
-  <si>
     <t>Kabira</t>
   </si>
   <si>
@@ -366,6 +285,81 @@
   </si>
   <si>
     <t>Senorita</t>
+  </si>
+  <si>
+    <t>Aaj Jaane Ki Zidd Na Karo</t>
+  </si>
+  <si>
+    <t>Aaoge Jab Tum</t>
+  </si>
+  <si>
+    <t>Saawali Si Raat</t>
+  </si>
+  <si>
+    <t>Phir Le Aya Dil</t>
+  </si>
+  <si>
+    <t>Itni Si Hasi</t>
+  </si>
+  <si>
+    <t>Main Kya Karoon</t>
+  </si>
+  <si>
+    <t>Kyon</t>
+  </si>
+  <si>
+    <t>Baatein Kuch Ankahee</t>
+  </si>
+  <si>
+    <t>Alvida</t>
+  </si>
+  <si>
+    <t>O Meri Jaan</t>
+  </si>
+  <si>
+    <t>In Dino</t>
+  </si>
+  <si>
+    <t>Tu Aashiqui Hai</t>
+  </si>
+  <si>
+    <t>Piyu Bole</t>
+  </si>
+  <si>
+    <t>Mitwa</t>
+  </si>
+  <si>
+    <t>Afreen Afreen</t>
+  </si>
+  <si>
+    <t>Bakhuda Tumhi Ho</t>
+  </si>
+  <si>
+    <t>Cheap Thrills</t>
+  </si>
+  <si>
+    <t>Khaabon Ke Parinday</t>
+  </si>
+  <si>
+    <t>Naina Da Kya Kasoor</t>
+  </si>
+  <si>
+    <t>Shubharambh</t>
+  </si>
+  <si>
+    <t>Manja</t>
+  </si>
+  <si>
+    <t>Duniya</t>
+  </si>
+  <si>
+    <t>Allah Ke Bande</t>
+  </si>
+  <si>
+    <t>Sajna Aa Bhi Ja</t>
+  </si>
+  <si>
+    <t>Naina</t>
   </si>
 </sst>
 </file>
@@ -732,8 +726,8 @@
   <dimension ref="A1:XEX37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
@@ -755,10 +749,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -772,10 +766,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -789,13 +783,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26.4">
@@ -806,523 +800,523 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="26.4">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="26.4">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="26.4">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="26.4">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26.4">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="26.4">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="26.4">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="26.4">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="26.4">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="26.4">
       <c r="A32" s="1" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="26.4">
       <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:5">

</xml_diff>